<commit_message>
Improve counter, add excel, add text preprocessing and add heatmap
</commit_message>
<xml_diff>
--- a/Threat reports.xlsx
+++ b/Threat reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.winters\NextCloud\Documents\Thesis\RQ1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.winters\Nextcloud\Documents\Thesis\Code\Threat-Report-Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA818800-3D79-43A7-B27A-48B1E4D5C4A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DEB87-AF29-4705-9D6F-DB78B758D797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Top cybersecurity companies" sheetId="1" r:id="rId1"/>
@@ -33,8 +33,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -305,9 +303,6 @@
     <t>quarter</t>
   </si>
   <si>
-    <t xml:space="preserve">adware, coinminers, ransomware, information stealers, remote access trojans, technical support cams, </t>
-  </si>
-  <si>
     <t>Q3/21 Threat report</t>
   </si>
   <si>
@@ -317,9 +312,6 @@
     <t>Gamaredon</t>
   </si>
   <si>
-    <t xml:space="preserve">coinminers, ransomware, rootkits, information stealers, remote access trojans, technical support cams, </t>
-  </si>
-  <si>
     <t>2020 YIR</t>
   </si>
   <si>
@@ -410,9 +402,6 @@
     <t>Cyber security threat trends</t>
   </si>
   <si>
-    <t>cryptominig, phishing, ransomware, trojans, botnet, remote access trojan, adware, exploit kit, information stealer</t>
-  </si>
-  <si>
     <t>Crowdstrike</t>
   </si>
   <si>
@@ -638,9 +627,6 @@
     <t>https://www.verizon.com/business/resources/reports/2021-data-breach-investigations-report.pdf</t>
   </si>
   <si>
-    <t>phishing, use of stolen credentials, ransomware, pretexting, misconfiguration, misdelivery, brute force, C2, backdoor, privilege abuse, capture app data, trojan, vulnerability exploitation, remote access trojans, information stealers, denial of service</t>
-  </si>
-  <si>
     <t>denial of service, phishing, loss, ransomware, C2, use of stolen credentials, pretexting, misconficuration, privilege abuse, trojan, password dumper, vulnerability exploitation, information stealer, capture app data</t>
   </si>
   <si>
@@ -690,6 +676,18 @@
   </si>
   <si>
     <t>Threat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">adware, coinminers, ransomware, information stealers, remote access trojan, technical support cams, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">coinminers, ransomware, rootkits, information stealers, remote access trojan, technical support cams, </t>
+  </si>
+  <si>
+    <t>cryptominig, phishing, ransomware, trojan, botnet, remote access trojan, adware, exploit kit, information stealer</t>
+  </si>
+  <si>
+    <t>phishing, use of stolen credentials, ransomware, pretexting, misconfiguration, misdelivery, brute force, C2, backdoor, privilege abuse, capture app data, trojan, vulnerability exploitation, remote access trojan, information stealers, denial of service</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1099,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -1110,7 +1108,7 @@
         <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1322,7 +1320,7 @@
         <v>35</v>
       </c>
       <c r="D18" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E18" t="b">
         <f>NOT(ISERROR(MATCH(A18,'Threat reports'!A:A,0)))</f>
@@ -1337,7 +1335,7 @@
         <v>35</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E19" t="b">
         <f>NOT(ISERROR(MATCH(A19,'Threat reports'!A:A,0)))</f>
@@ -1400,7 +1398,7 @@
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="E24" t="b">
         <f>NOT(ISERROR(MATCH(A24,'Threat reports'!A:A,0)))</f>
@@ -1427,7 +1425,7 @@
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E26" t="b">
         <f>NOT(ISERROR(MATCH(A26,'Threat reports'!A:A,0)))</f>
@@ -1478,7 +1476,7 @@
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="E30" t="b">
         <f>NOT(ISERROR(MATCH(A30,'Threat reports'!A:A,0)))</f>
@@ -1493,7 +1491,7 @@
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E31" t="b">
         <f>NOT(ISERROR(MATCH(A31,'Threat reports'!A:A,0)))</f>
@@ -1544,7 +1542,7 @@
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E35" t="b">
         <f>NOT(ISERROR(MATCH(A35,'Threat reports'!A:A,0)))</f>
@@ -1577,7 +1575,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -1595,7 +1593,7 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E39" t="b">
         <f>NOT(ISERROR(MATCH(A39,'Threat reports'!A:A,0)))</f>
@@ -1622,7 +1620,7 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E41" t="b">
         <f>NOT(ISERROR(MATCH(A41,'Threat reports'!A:A,0)))</f>
@@ -1661,7 +1659,7 @@
         <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E44" t="b">
         <f>NOT(ISERROR(MATCH(A44,'Threat reports'!A:A,0)))</f>
@@ -1712,7 +1710,7 @@
         <v>35</v>
       </c>
       <c r="D48" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="E48" t="b">
         <f>NOT(ISERROR(MATCH(A48,'Threat reports'!A:A,0)))</f>
@@ -1727,7 +1725,7 @@
         <v>35</v>
       </c>
       <c r="D49" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E49" t="b">
         <f>NOT(ISERROR(MATCH(A49,'Threat reports'!A:A,0)))</f>
@@ -1800,7 +1798,7 @@
         <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1896,8 +1894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
   <dimension ref="A1:J35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1919,7 +1917,7 @@
         <v>75</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>86</v>
@@ -1931,13 +1929,13 @@
         <v>77</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1957,7 +1955,7 @@
         <v>82</v>
       </c>
       <c r="I2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1977,13 +1975,13 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
-        <v>87</v>
+        <v>212</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
       </c>
       <c r="I3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1991,10 +1989,10 @@
         <v>8</v>
       </c>
       <c r="B4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="D4">
         <v>2021</v>
@@ -2003,13 +2001,13 @@
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>213</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -2017,19 +2015,19 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D5">
         <v>2020</v>
       </c>
       <c r="F5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -2037,16 +2035,16 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D6">
         <v>2022</v>
       </c>
       <c r="I6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -2054,25 +2052,25 @@
         <v>26</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D7">
         <v>2020</v>
       </c>
       <c r="F7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -2080,25 +2078,25 @@
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>2021</v>
       </c>
       <c r="F8" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -2106,22 +2104,22 @@
         <v>28</v>
       </c>
       <c r="B9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9">
         <v>2021</v>
       </c>
       <c r="F9" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="I9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="J9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -2129,16 +2127,16 @@
         <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D10">
         <v>2022</v>
       </c>
       <c r="J10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -2146,16 +2144,16 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11">
         <v>2021</v>
       </c>
       <c r="J11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -2163,59 +2161,59 @@
         <v>5</v>
       </c>
       <c r="B12" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D12">
         <v>2020</v>
       </c>
       <c r="F12" t="s">
-        <v>122</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B13" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D13">
         <v>2021</v>
       </c>
       <c r="F13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G13" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="H13" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D14">
         <v>2020</v>
       </c>
       <c r="J14" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -2223,16 +2221,16 @@
         <v>39</v>
       </c>
       <c r="B15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C15" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D15">
         <v>2021</v>
       </c>
       <c r="F15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -2240,16 +2238,16 @@
         <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C16" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="D16">
         <v>2022</v>
       </c>
       <c r="F16" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -2257,25 +2255,25 @@
         <v>29</v>
       </c>
       <c r="B17" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C17" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D17">
         <v>2021</v>
       </c>
       <c r="F17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="G17" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="I17" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -2283,10 +2281,10 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C18" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D18">
         <v>2021</v>
@@ -2295,16 +2293,16 @@
         <v>1.2</v>
       </c>
       <c r="F18" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="G18" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="I18" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J18" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -2312,10 +2310,10 @@
         <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D19">
         <v>2021</v>
@@ -2324,13 +2322,13 @@
         <v>3.4</v>
       </c>
       <c r="F19" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="I19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J19" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
@@ -2338,10 +2336,10 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C20" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D20">
         <v>2022</v>
@@ -2350,16 +2348,16 @@
         <v>1.2</v>
       </c>
       <c r="F20" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G20" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="I20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="J20" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
@@ -2367,22 +2365,22 @@
         <v>2</v>
       </c>
       <c r="B21" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C21" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D21">
         <v>2021</v>
       </c>
       <c r="F21" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G21" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="I21" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
@@ -2390,22 +2388,22 @@
         <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D22">
         <v>2020</v>
       </c>
       <c r="F22" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G22" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I22" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
@@ -2413,22 +2411,22 @@
         <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C23" t="s">
+        <v>157</v>
+      </c>
+      <c r="D23" t="s">
         <v>160</v>
       </c>
-      <c r="D23" t="s">
+      <c r="F23" t="s">
         <v>163</v>
       </c>
-      <c r="F23" t="s">
-        <v>166</v>
-      </c>
       <c r="G23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="I23" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
@@ -2436,22 +2434,22 @@
         <v>13</v>
       </c>
       <c r="B24" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C24" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D24">
         <v>2021</v>
       </c>
       <c r="F24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="G24" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="I24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
@@ -2459,22 +2457,22 @@
         <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C25" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D25">
         <v>2020</v>
       </c>
       <c r="F25" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="G25" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="I25" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
@@ -2482,16 +2480,16 @@
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D26">
         <v>2022</v>
       </c>
       <c r="F26" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="I26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
@@ -2499,13 +2497,13 @@
         <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C27" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="J27" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
@@ -2513,19 +2511,19 @@
         <v>15</v>
       </c>
       <c r="B28" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C28" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D28">
         <v>2022</v>
       </c>
       <c r="F28" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="G28" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
@@ -2533,19 +2531,19 @@
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C29" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="D29">
         <v>2021</v>
       </c>
       <c r="F29" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G29" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
@@ -2553,16 +2551,16 @@
         <v>15</v>
       </c>
       <c r="B30" t="s">
+        <v>178</v>
+      </c>
+      <c r="C30" t="s">
         <v>181</v>
-      </c>
-      <c r="C30" t="s">
-        <v>184</v>
       </c>
       <c r="D30">
         <v>2020</v>
       </c>
       <c r="F30" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
@@ -2570,16 +2568,16 @@
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C31" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="D31">
         <v>2020</v>
       </c>
       <c r="F31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
@@ -2587,19 +2585,19 @@
         <v>48</v>
       </c>
       <c r="B32" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C32" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D32">
         <v>2021</v>
       </c>
       <c r="F32" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="J32" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
@@ -2607,30 +2605,30 @@
         <v>49</v>
       </c>
       <c r="B33" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="D33">
         <v>2022</v>
       </c>
       <c r="F33" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="I33" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="C34" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D34">
         <v>2021</v>
       </c>
       <c r="F34" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
@@ -2638,7 +2636,7 @@
         <v>2020</v>
       </c>
       <c r="F35" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -2664,7 +2662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51753539-79C4-4240-92CD-110E12249F67}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -2678,18 +2676,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C2" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add time coverage for reports
</commit_message>
<xml_diff>
--- a/Threat reports.xlsx
+++ b/Threat reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.winters\Nextcloud\Documents\Thesis\Code\Threat-Report-Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966DEB87-AF29-4705-9D6F-DB78B758D797}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC2542D-851E-4329-B14F-8501B15BD93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Top cybersecurity companies" sheetId="1" r:id="rId1"/>
@@ -19,6 +19,7 @@
     <sheet name="Synonyms" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Threat reports'!$A$1:$J$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Top cybersecurity companies'!$A$1:$C$49</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="216">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="220">
   <si>
     <t>Name</t>
   </si>
@@ -688,6 +689,18 @@
   </si>
   <si>
     <t>phishing, use of stolen credentials, ransomware, pretexting, misconfiguration, misdelivery, brute force, C2, backdoor, privilege abuse, capture app data, trojan, vulnerability exploitation, remote access trojan, information stealers, denial of service</t>
+  </si>
+  <si>
+    <t>2021-4</t>
+  </si>
+  <si>
+    <t>2021-3</t>
+  </si>
+  <si>
+    <t>2021-1, 2021-2</t>
+  </si>
+  <si>
+    <t>2021-3, 2021-4</t>
   </si>
 </sst>
 </file>
@@ -1892,10 +1905,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1903,6 +1917,8 @@
     <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.88671875" customWidth="1"/>
     <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1971,8 +1987,8 @@
       <c r="D3">
         <v>2021</v>
       </c>
-      <c r="E3">
-        <v>4</v>
+      <c r="E3" t="s">
+        <v>216</v>
       </c>
       <c r="F3" t="s">
         <v>212</v>
@@ -1997,8 +2013,8 @@
       <c r="D4">
         <v>2021</v>
       </c>
-      <c r="E4">
-        <v>3</v>
+      <c r="E4" t="s">
+        <v>217</v>
       </c>
       <c r="F4" t="s">
         <v>213</v>
@@ -2010,7 +2026,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2030,7 +2046,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2047,7 +2063,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2122,7 +2138,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2156,7 +2172,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2199,7 +2215,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2233,7 +2249,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2289,8 +2305,8 @@
       <c r="D18">
         <v>2021</v>
       </c>
-      <c r="E18">
-        <v>1.2</v>
+      <c r="E18" t="s">
+        <v>218</v>
       </c>
       <c r="F18" t="s">
         <v>145</v>
@@ -2318,8 +2334,8 @@
       <c r="D19">
         <v>2021</v>
       </c>
-      <c r="E19">
-        <v>3.4</v>
+      <c r="E19" t="s">
+        <v>219</v>
       </c>
       <c r="F19" t="s">
         <v>197</v>
@@ -2331,7 +2347,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2383,7 +2399,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2452,7 +2468,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2475,7 +2491,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2506,7 +2522,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2546,7 +2562,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2563,7 +2579,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2600,7 +2616,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2631,7 +2647,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
       <c r="D35">
         <v>2020</v>
       </c>
@@ -2640,6 +2656,14 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J35" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
+    <filterColumn colId="3">
+      <filters blank="1">
+        <filter val="2021"/>
+        <filter val="2021/2022"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{2BC7DD5D-A004-4919-9154-D6F987ACE33C}"/>

</xml_diff>

<commit_message>
Remove duplicate actors and ttps (groupby)
</commit_message>
<xml_diff>
--- a/Threat reports.xlsx
+++ b/Threat reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.winters\Nextcloud\Documents\Thesis\Code\Threat-Report-Analyzer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kingpolis-my.sharepoint.com/personal/abe_winters_kingpolis_nl/Documents/Documenten/Studie/Threat-Report-Analyzer/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CC2542D-851E-4329-B14F-8501B15BD93A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{8CC2542D-851E-4329-B14F-8501B15BD93A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BFEE5F8-378C-476A-81EB-37DC2E67569D}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Top cybersecurity companies" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="230">
   <si>
     <t>Name</t>
   </si>
@@ -701,6 +701,36 @@
   </si>
   <si>
     <t>2021-3, 2021-4</t>
+  </si>
+  <si>
+    <t>2021-1, 2021-2, 2021-3, 2021-4</t>
+  </si>
+  <si>
+    <t>Accenture</t>
+  </si>
+  <si>
+    <t>2021-1, 2021-2, 2021-3</t>
+  </si>
+  <si>
+    <t>predicts landscape for 2021</t>
+  </si>
+  <si>
+    <t>2021-3, 2021-4, 2022-1, 2022-2</t>
+  </si>
+  <si>
+    <t>ENISA Threat Landscape 2022</t>
+  </si>
+  <si>
+    <t>Google Threat Analysis Group</t>
+  </si>
+  <si>
+    <t>APT40, Gamaredon, Lazarus, Sandworm, APT28, APT41, Nobelium, Ghostwriter, Moses Staff, Black Shadow, TeamTNT, REvil, Cl0p, NetWalker, LockerGoga,  MegaCortex, BlackCat, Conti, DEV-0537, Karakurt, DeathStalker, Candiru, Anonymous, TeamOneFirst, GhostSec, Against The West, NB65, Belarusian Cyber Partisans, KILLNET, XakNet, The Red Bandits</t>
+  </si>
+  <si>
+    <t>2020-1, 2020-2, 2020-3, 2020-4</t>
+  </si>
+  <si>
+    <t>2021-2, 2021-3, 2021-4, 2022-1</t>
   </si>
 </sst>
 </file>
@@ -766,7 +796,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -797,7 +827,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1093,21 +1123,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49E475BD-DDED-4FBF-B8E6-D88C8705447F}">
-  <dimension ref="A1:E49"/>
+  <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.109375" customWidth="1"/>
-    <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.08984375" customWidth="1"/>
+    <col min="4" max="4" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1124,7 +1154,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1139,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1154,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1169,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1181,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1193,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1205,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1229,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1241,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1253,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1277,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1289,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1301,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1313,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1325,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1340,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1355,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1379,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1391,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1403,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1418,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1430,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1445,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1457,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1469,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1481,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1496,7 +1526,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1511,7 +1541,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1523,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1535,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1547,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1562,7 +1592,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1574,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1586,7 +1616,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>174</v>
       </c>
@@ -1598,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1613,7 +1643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1625,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1640,7 +1670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1652,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1664,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1679,7 +1709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1691,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1703,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1715,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1730,7 +1760,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1743,6 +1773,11 @@
       <c r="E49" t="b">
         <f>NOT(ISERROR(MATCH(A49,'Threat reports'!A:A,0)))</f>
         <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -1768,13 +1803,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1785,7 +1820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1793,17 +1828,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1814,82 +1849,82 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>72</v>
       </c>
@@ -1905,24 +1940,23 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:J35"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="9.77734375" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.90625" customWidth="1"/>
+    <col min="3" max="3" width="45.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.81640625" customWidth="1"/>
+    <col min="6" max="6" width="18.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1954,7 +1988,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1974,7 +2008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2000,7 +2034,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +2060,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2046,7 +2080,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2063,7 +2097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2089,7 +2123,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2102,6 +2136,9 @@
       <c r="D8">
         <v>2021</v>
       </c>
+      <c r="E8" t="s">
+        <v>220</v>
+      </c>
       <c r="F8" t="s">
         <v>200</v>
       </c>
@@ -2115,7 +2152,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2128,6 +2165,9 @@
       <c r="D9">
         <v>2021</v>
       </c>
+      <c r="E9" t="s">
+        <v>222</v>
+      </c>
       <c r="F9" t="s">
         <v>201</v>
       </c>
@@ -2138,7 +2178,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2155,7 +2195,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2172,7 +2212,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2189,7 +2229,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2202,6 +2242,9 @@
       <c r="D13">
         <v>2021</v>
       </c>
+      <c r="E13" t="s">
+        <v>220</v>
+      </c>
       <c r="F13" t="s">
         <v>124</v>
       </c>
@@ -2215,7 +2258,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2232,7 +2275,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2248,8 +2291,11 @@
       <c r="F15" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2266,7 +2312,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2279,6 +2325,9 @@
       <c r="D17">
         <v>2021</v>
       </c>
+      <c r="E17" t="s">
+        <v>220</v>
+      </c>
       <c r="F17" t="s">
         <v>138</v>
       </c>
@@ -2292,7 +2341,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2321,7 +2370,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2347,7 +2396,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2360,8 +2409,8 @@
       <c r="D20">
         <v>2022</v>
       </c>
-      <c r="E20">
-        <v>1.2</v>
+      <c r="E20" t="s">
+        <v>218</v>
       </c>
       <c r="F20" t="s">
         <v>203</v>
@@ -2376,7 +2425,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2389,6 +2438,9 @@
       <c r="D21">
         <v>2021</v>
       </c>
+      <c r="E21" t="s">
+        <v>220</v>
+      </c>
       <c r="F21" t="s">
         <v>204</v>
       </c>
@@ -2399,7 +2451,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2422,7 +2474,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2445,7 +2497,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2458,6 +2510,9 @@
       <c r="D24">
         <v>2021</v>
       </c>
+      <c r="E24" t="s">
+        <v>222</v>
+      </c>
       <c r="F24" t="s">
         <v>163</v>
       </c>
@@ -2468,7 +2523,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2491,7 +2546,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>11</v>
       </c>
@@ -2499,7 +2554,10 @@
         <v>168</v>
       </c>
       <c r="D26">
-        <v>2022</v>
+        <v>2021</v>
+      </c>
+      <c r="E26" t="s">
+        <v>229</v>
       </c>
       <c r="F26" t="s">
         <v>169</v>
@@ -2508,7 +2566,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -2522,7 +2580,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>15</v>
       </c>
@@ -2542,7 +2600,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>15</v>
       </c>
@@ -2562,7 +2620,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="30" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -2579,7 +2637,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="31" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>46</v>
       </c>
@@ -2596,7 +2654,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -2609,6 +2667,9 @@
       <c r="D32">
         <v>2021</v>
       </c>
+      <c r="E32" t="s">
+        <v>220</v>
+      </c>
       <c r="F32" t="s">
         <v>191</v>
       </c>
@@ -2616,7 +2677,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2627,7 +2688,10 @@
         <v>193</v>
       </c>
       <c r="D33">
-        <v>2022</v>
+        <v>2021</v>
+      </c>
+      <c r="E33" t="s">
+        <v>220</v>
       </c>
       <c r="F33" t="s">
         <v>199</v>
@@ -2636,34 +2700,64 @@
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>49</v>
+      </c>
+      <c r="B34" t="s">
+        <v>134</v>
+      </c>
       <c r="C34" t="s">
         <v>194</v>
       </c>
       <c r="D34">
-        <v>2021</v>
+        <v>2020</v>
+      </c>
+      <c r="E34" t="s">
+        <v>228</v>
       </c>
       <c r="F34" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>49</v>
+      </c>
+      <c r="B35" t="s">
+        <v>134</v>
+      </c>
       <c r="D35">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F35" t="s">
         <v>195</v>
       </c>
     </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>50</v>
+      </c>
+      <c r="B36" t="s">
+        <v>225</v>
+      </c>
+      <c r="D36">
+        <v>2021</v>
+      </c>
+      <c r="E36" t="s">
+        <v>224</v>
+      </c>
+      <c r="G36" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>226</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J35" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
-    <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="2021"/>
-        <filter val="2021/2022"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J35" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{2BC7DD5D-A004-4919-9154-D6F987ACE33C}"/>
@@ -2690,9 +2784,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2703,7 +2797,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>211</v>
       </c>

</xml_diff>

<commit_message>
Improve method 3 usability
</commit_message>
<xml_diff>
--- a/Threat reports.xlsx
+++ b/Threat reports.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kingpolis-my.sharepoint.com/personal/abe_winters_kingpolis_nl/Documents/Documenten/Studie/Threat-Report-Analyzer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\a.winters\Nextcloud\Documents\Thesis\Code\Threat-Report-Analyzer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="13_ncr:1_{8CC2542D-851E-4329-B14F-8501B15BD93A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BFEE5F8-378C-476A-81EB-37DC2E67569D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20E4E8EE-9693-412B-9397-96B0794ACB1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{6F1AC249-628C-46B2-AC53-6AD59A257E7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Top cybersecurity companies" sheetId="1" r:id="rId1"/>
@@ -538,9 +538,6 @@
     <t>APT29, Fancy Bear, Callisto Group, Sandworm, Gamaredon, Energetic Bear, SoftCell, APT15, APT40, APT38, Lazarus, Konni, Andariel, Tortoiseshell, Charming Kitten</t>
   </si>
   <si>
-    <t>Tortoiseshell, Charming Kitten, Fox Kitten Parasite, ControlX, APT40, APT5, APT15, APT31, Sea Turtle, Kimsuky, Konni, Lazarus, APT32, Energetic Bear, UNC2452, APT28</t>
-  </si>
-  <si>
     <t>Has web application report and malware analysis report, no (global) threat report. Web application report is on unsecure file uploads</t>
   </si>
   <si>
@@ -731,6 +728,9 @@
   </si>
   <si>
     <t>2021-2, 2021-3, 2021-4, 2022-1</t>
+  </si>
+  <si>
+    <t>Tortoiseshell, Charming Kitten, Fox Kitten Parasite, ControlX, APT40, APT5, APT15, APT31, Sea Turtle, Kimsuky, Konni, Lazarus, APT32, Energetic Bear, UNC2452, APT28, Nobelium, Hafnium, Nickel, Thallium, Phosphorus, Cerium, Gadolinium, Strontium, Bromine</t>
   </si>
 </sst>
 </file>
@@ -796,7 +796,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -827,7 +827,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1129,20 +1129,20 @@
       <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.08984375" customWidth="1"/>
-    <col min="4" max="4" width="36.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.109375" customWidth="1"/>
+    <col min="4" max="4" width="36.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>34</v>
@@ -1154,7 +1154,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>20</v>
       </c>
@@ -1169,7 +1169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1184,7 +1184,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1199,7 +1199,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1211,7 +1211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1223,7 +1223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>28</v>
       </c>
@@ -1235,7 +1235,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1247,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>21</v>
       </c>
@@ -1259,7 +1259,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -1271,7 +1271,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>45</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -1295,7 +1295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>39</v>
       </c>
@@ -1307,7 +1307,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>4</v>
       </c>
@@ -1319,7 +1319,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1370,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>27</v>
       </c>
@@ -1385,7 +1385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1397,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>31</v>
       </c>
@@ -1409,7 +1409,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>36</v>
       </c>
@@ -1421,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1433,7 +1433,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1448,7 +1448,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -1460,7 +1460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>3</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>13</v>
       </c>
@@ -1499,7 +1499,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>44</v>
       </c>
@@ -1511,7 +1511,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -1519,14 +1519,14 @@
         <v>35</v>
       </c>
       <c r="D30" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E30" t="b">
         <f>NOT(ISERROR(MATCH(A30,'Threat reports'!A:A,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>11</v>
       </c>
@@ -1534,14 +1534,14 @@
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E31" t="b">
         <f>NOT(ISERROR(MATCH(A31,'Threat reports'!A:A,0)))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>19</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>24</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>12</v>
       </c>
@@ -1577,7 +1577,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>37</v>
       </c>
@@ -1585,14 +1585,14 @@
         <v>35</v>
       </c>
       <c r="D35" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E35" t="b">
         <f>NOT(ISERROR(MATCH(A35,'Threat reports'!A:A,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>1</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>32</v>
       </c>
@@ -1616,9 +1616,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
         <v>35</v>
@@ -1628,7 +1628,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>14</v>
       </c>
@@ -1636,14 +1636,14 @@
         <v>35</v>
       </c>
       <c r="D39" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="E39" t="b">
         <f>NOT(ISERROR(MATCH(A39,'Threat reports'!A:A,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1663,14 +1663,14 @@
         <v>35</v>
       </c>
       <c r="D41" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E41" t="b">
         <f>NOT(ISERROR(MATCH(A41,'Threat reports'!A:A,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>9</v>
       </c>
@@ -1682,7 +1682,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -1694,7 +1694,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>38</v>
       </c>
@@ -1702,14 +1702,14 @@
         <v>35</v>
       </c>
       <c r="D44" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="E44" t="b">
         <f>NOT(ISERROR(MATCH(A44,'Threat reports'!A:A,0)))</f>
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>15</v>
       </c>
@@ -1721,7 +1721,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -1733,7 +1733,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -1745,7 +1745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -1753,14 +1753,14 @@
         <v>35</v>
       </c>
       <c r="D48" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E48" t="b">
         <f>NOT(ISERROR(MATCH(A48,'Threat reports'!A:A,0)))</f>
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -1775,9 +1775,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1803,13 +1803,13 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>50</v>
       </c>
@@ -1828,17 +1828,17 @@
         <v>53</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>73</v>
       </c>
@@ -1846,85 +1846,85 @@
         <v>57</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B12" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B15" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
         <v>72</v>
       </c>
@@ -1942,21 +1942,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2689BB-6B93-4C75-AE6B-11DC67E6D6D5}">
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.90625" customWidth="1"/>
-    <col min="3" max="3" width="45.54296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" customWidth="1"/>
-    <col min="6" max="6" width="18.6328125" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="45.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>74</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -2008,7 +2008,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -2022,10 +2022,10 @@
         <v>2021</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G3" t="s">
         <v>85</v>
@@ -2034,7 +2034,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -2048,10 +2048,10 @@
         <v>2021</v>
       </c>
       <c r="E4" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="F4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G4" t="s">
         <v>89</v>
@@ -2060,7 +2060,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2080,7 +2080,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -2123,7 +2123,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -2137,10 +2137,10 @@
         <v>2021</v>
       </c>
       <c r="E8" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G8" t="s">
         <v>109</v>
@@ -2152,7 +2152,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -2166,10 +2166,10 @@
         <v>2021</v>
       </c>
       <c r="E9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F9" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="I9" t="s">
         <v>107</v>
@@ -2178,7 +2178,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -2195,7 +2195,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>21</v>
       </c>
@@ -2212,7 +2212,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>5</v>
       </c>
@@ -2226,10 +2226,10 @@
         <v>2020</v>
       </c>
       <c r="F12" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>120</v>
       </c>
@@ -2243,7 +2243,7 @@
         <v>2021</v>
       </c>
       <c r="E13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F13" t="s">
         <v>124</v>
@@ -2258,7 +2258,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2275,7 +2275,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>39</v>
       </c>
@@ -2292,10 +2292,10 @@
         <v>131</v>
       </c>
       <c r="J15" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>4</v>
       </c>
@@ -2309,10 +2309,10 @@
         <v>2022</v>
       </c>
       <c r="F16" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>29</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>2021</v>
       </c>
       <c r="E17" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F17" t="s">
         <v>138</v>
@@ -2341,7 +2341,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2355,7 +2355,7 @@
         <v>2021</v>
       </c>
       <c r="E18" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F18" t="s">
         <v>145</v>
@@ -2370,7 +2370,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>16</v>
       </c>
@@ -2384,10 +2384,10 @@
         <v>2021</v>
       </c>
       <c r="E19" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="F19" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I19" t="s">
         <v>108</v>
@@ -2396,7 +2396,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2410,10 +2410,10 @@
         <v>2022</v>
       </c>
       <c r="E20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="F20" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G20" t="s">
         <v>146</v>
@@ -2425,7 +2425,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2439,10 +2439,10 @@
         <v>2021</v>
       </c>
       <c r="E21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G21" t="s">
         <v>154</v>
@@ -2451,7 +2451,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2474,7 +2474,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>13</v>
       </c>
@@ -2511,19 +2511,19 @@
         <v>2021</v>
       </c>
       <c r="E24" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="F24" t="s">
         <v>163</v>
       </c>
       <c r="G24" t="s">
-        <v>165</v>
+        <v>229</v>
       </c>
       <c r="I24" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -2537,7 +2537,7 @@
         <v>2020</v>
       </c>
       <c r="F25" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G25" t="s">
         <v>162</v>
@@ -2546,138 +2546,138 @@
         <v>108</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>11</v>
       </c>
       <c r="C26" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D26">
         <v>2021</v>
       </c>
       <c r="E26" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="F26" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="I26" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>32</v>
       </c>
       <c r="B27" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" t="s">
         <v>172</v>
       </c>
-      <c r="C27" t="s">
-        <v>173</v>
-      </c>
       <c r="J27" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>15</v>
       </c>
       <c r="B28" t="s">
+        <v>177</v>
+      </c>
+      <c r="C28" t="s">
         <v>178</v>
-      </c>
-      <c r="C28" t="s">
-        <v>179</v>
       </c>
       <c r="D28">
         <v>2022</v>
       </c>
       <c r="F28" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G28" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>15</v>
       </c>
       <c r="B29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C29" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D29">
         <v>2021</v>
       </c>
       <c r="F29" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="G29" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C30" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D30">
         <v>2020</v>
       </c>
       <c r="F30" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C31" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D31">
         <v>2020</v>
       </c>
       <c r="F31" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>48</v>
       </c>
       <c r="B32" t="s">
+        <v>188</v>
+      </c>
+      <c r="C32" t="s">
         <v>189</v>
-      </c>
-      <c r="C32" t="s">
-        <v>190</v>
       </c>
       <c r="D32">
         <v>2021</v>
       </c>
       <c r="E32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F32" t="s">
+        <v>190</v>
+      </c>
+      <c r="J32" t="s">
         <v>191</v>
       </c>
-      <c r="J32" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -2685,22 +2685,22 @@
         <v>134</v>
       </c>
       <c r="C33" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D33">
         <v>2021</v>
       </c>
       <c r="E33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F33" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="I33" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>49</v>
       </c>
@@ -2708,19 +2708,19 @@
         <v>134</v>
       </c>
       <c r="C34" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D34">
         <v>2020</v>
       </c>
       <c r="E34" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="F34" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>49</v>
       </c>
@@ -2731,29 +2731,29 @@
         <v>2019</v>
       </c>
       <c r="F35" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>50</v>
       </c>
       <c r="B36" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D36">
         <v>2021</v>
       </c>
       <c r="E36" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="G36" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
   </sheetData>
@@ -2784,9 +2784,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
@@ -2794,18 +2794,18 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>209</v>
-      </c>
-      <c r="C2" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>